<commit_message>
Commiting changes to run as Maven suite using Surefire plugin
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/testdata.xlsx
+++ b/src/test/resources/Excel/testdata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naisha Jain\workspace\ootbsuite\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189CB572-4A06-451A-AC27-782623233463}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22AC21FA-FE98-426B-AF3E-132C0839C9F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -532,7 +532,7 @@
         <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>34</v>

</xml_diff>